<commit_message>
new adjusted Gannt chart
</commit_message>
<xml_diff>
--- a/doc/project Gannt Chart.xlsx
+++ b/doc/project Gannt Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric Xue\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2C110B-7A21-4B21-A7F2-55797E74ECDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81987F88-E750-4CEA-BAAA-DCC1F6BFB1E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="585" windowWidth="18000" windowHeight="9165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Project name</t>
   </si>
@@ -90,6 +90,18 @@
   </si>
   <si>
     <t>debugg before final submission</t>
+  </si>
+  <si>
+    <t>unit tests</t>
+  </si>
+  <si>
+    <t>package the project</t>
+  </si>
+  <si>
+    <t>feature: file selection interface</t>
+  </si>
+  <si>
+    <t>tutorial notebook</t>
   </si>
 </sst>
 </file>
@@ -114,7 +126,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,6 +169,30 @@
         <bgColor rgb="FFF6B26B"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -170,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -186,12 +222,23 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF9966FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -404,23 +451,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:CN11"/>
+  <dimension ref="A1:EU15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
     <col min="3" max="3" width="8.140625" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" customWidth="1"/>
     <col min="5" max="5" width="5.5703125" customWidth="1"/>
-    <col min="6" max="92" width="2.5703125" customWidth="1"/>
+    <col min="6" max="151" width="2.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:92" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:151" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -434,7 +481,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:92" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:151" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C2" s="2">
         <v>45380</v>
       </c>
@@ -442,7 +489,7 @@
         <v>45450</v>
       </c>
     </row>
-    <row r="4" spans="1:92" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:151" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -782,26 +829,280 @@
         <f t="shared" si="0"/>
         <v>45460</v>
       </c>
-      <c r="CI4" s="3"/>
-      <c r="CJ4" s="3"/>
-      <c r="CK4" s="3"/>
-      <c r="CL4" s="3"/>
-      <c r="CM4" s="3"/>
-      <c r="CN4" s="3"/>
+      <c r="CI4" s="3">
+        <f t="shared" ref="CI4" si="1">CH4+1</f>
+        <v>45461</v>
+      </c>
+      <c r="CJ4" s="3">
+        <f t="shared" ref="CJ4" si="2">CI4+1</f>
+        <v>45462</v>
+      </c>
+      <c r="CK4" s="3">
+        <f t="shared" ref="CK4" si="3">CJ4+1</f>
+        <v>45463</v>
+      </c>
+      <c r="CL4" s="3">
+        <f t="shared" ref="CL4" si="4">CK4+1</f>
+        <v>45464</v>
+      </c>
+      <c r="CM4" s="3">
+        <f t="shared" ref="CM4" si="5">CL4+1</f>
+        <v>45465</v>
+      </c>
+      <c r="CN4" s="3">
+        <f t="shared" ref="CN4" si="6">CM4+1</f>
+        <v>45466</v>
+      </c>
+      <c r="CO4" s="3">
+        <f t="shared" ref="CO4" si="7">CN4+1</f>
+        <v>45467</v>
+      </c>
+      <c r="CP4" s="3">
+        <f t="shared" ref="CP4" si="8">CO4+1</f>
+        <v>45468</v>
+      </c>
+      <c r="CQ4" s="3">
+        <f t="shared" ref="CQ4" si="9">CP4+1</f>
+        <v>45469</v>
+      </c>
+      <c r="CR4" s="3">
+        <f t="shared" ref="CR4" si="10">CQ4+1</f>
+        <v>45470</v>
+      </c>
+      <c r="CS4" s="3">
+        <f t="shared" ref="CS4" si="11">CR4+1</f>
+        <v>45471</v>
+      </c>
+      <c r="CT4" s="3">
+        <f t="shared" ref="CT4" si="12">CS4+1</f>
+        <v>45472</v>
+      </c>
+      <c r="CU4" s="3">
+        <f t="shared" ref="CU4" si="13">CT4+1</f>
+        <v>45473</v>
+      </c>
+      <c r="CV4" s="3">
+        <f t="shared" ref="CV4" si="14">CU4+1</f>
+        <v>45474</v>
+      </c>
+      <c r="CW4" s="3">
+        <f t="shared" ref="CW4" si="15">CV4+1</f>
+        <v>45475</v>
+      </c>
+      <c r="CX4" s="3">
+        <f t="shared" ref="CX4" si="16">CW4+1</f>
+        <v>45476</v>
+      </c>
+      <c r="CY4" s="3">
+        <f t="shared" ref="CY4" si="17">CX4+1</f>
+        <v>45477</v>
+      </c>
+      <c r="CZ4" s="3">
+        <f t="shared" ref="CZ4" si="18">CY4+1</f>
+        <v>45478</v>
+      </c>
+      <c r="DA4" s="3">
+        <f t="shared" ref="DA4" si="19">CZ4+1</f>
+        <v>45479</v>
+      </c>
+      <c r="DB4" s="3">
+        <f t="shared" ref="DB4" si="20">DA4+1</f>
+        <v>45480</v>
+      </c>
+      <c r="DC4" s="3">
+        <f t="shared" ref="DC4" si="21">DB4+1</f>
+        <v>45481</v>
+      </c>
+      <c r="DD4" s="3">
+        <f t="shared" ref="DD4" si="22">DC4+1</f>
+        <v>45482</v>
+      </c>
+      <c r="DE4" s="3">
+        <f t="shared" ref="DE4" si="23">DD4+1</f>
+        <v>45483</v>
+      </c>
+      <c r="DF4" s="3">
+        <f t="shared" ref="DF4" si="24">DE4+1</f>
+        <v>45484</v>
+      </c>
+      <c r="DG4" s="3">
+        <f t="shared" ref="DG4" si="25">DF4+1</f>
+        <v>45485</v>
+      </c>
+      <c r="DH4" s="3">
+        <f t="shared" ref="DH4" si="26">DG4+1</f>
+        <v>45486</v>
+      </c>
+      <c r="DI4" s="3">
+        <f t="shared" ref="DI4" si="27">DH4+1</f>
+        <v>45487</v>
+      </c>
+      <c r="DJ4" s="3">
+        <f t="shared" ref="DJ4" si="28">DI4+1</f>
+        <v>45488</v>
+      </c>
+      <c r="DK4" s="3">
+        <f t="shared" ref="DK4" si="29">DJ4+1</f>
+        <v>45489</v>
+      </c>
+      <c r="DL4" s="3">
+        <f t="shared" ref="DL4" si="30">DK4+1</f>
+        <v>45490</v>
+      </c>
+      <c r="DM4" s="3">
+        <f t="shared" ref="DM4" si="31">DL4+1</f>
+        <v>45491</v>
+      </c>
+      <c r="DN4" s="3">
+        <f t="shared" ref="DN4" si="32">DM4+1</f>
+        <v>45492</v>
+      </c>
+      <c r="DO4" s="3">
+        <f t="shared" ref="DO4" si="33">DN4+1</f>
+        <v>45493</v>
+      </c>
+      <c r="DP4" s="3">
+        <f t="shared" ref="DP4" si="34">DO4+1</f>
+        <v>45494</v>
+      </c>
+      <c r="DQ4" s="3">
+        <f t="shared" ref="DQ4" si="35">DP4+1</f>
+        <v>45495</v>
+      </c>
+      <c r="DR4" s="3">
+        <f t="shared" ref="DR4" si="36">DQ4+1</f>
+        <v>45496</v>
+      </c>
+      <c r="DS4" s="3">
+        <f t="shared" ref="DS4" si="37">DR4+1</f>
+        <v>45497</v>
+      </c>
+      <c r="DT4" s="3">
+        <f t="shared" ref="DT4" si="38">DS4+1</f>
+        <v>45498</v>
+      </c>
+      <c r="DU4" s="3">
+        <f t="shared" ref="DU4" si="39">DT4+1</f>
+        <v>45499</v>
+      </c>
+      <c r="DV4" s="3">
+        <f t="shared" ref="DV4" si="40">DU4+1</f>
+        <v>45500</v>
+      </c>
+      <c r="DW4" s="3">
+        <f t="shared" ref="DW4" si="41">DV4+1</f>
+        <v>45501</v>
+      </c>
+      <c r="DX4" s="3">
+        <f t="shared" ref="DX4" si="42">DW4+1</f>
+        <v>45502</v>
+      </c>
+      <c r="DY4" s="3">
+        <f t="shared" ref="DY4" si="43">DX4+1</f>
+        <v>45503</v>
+      </c>
+      <c r="DZ4" s="3">
+        <f t="shared" ref="DZ4" si="44">DY4+1</f>
+        <v>45504</v>
+      </c>
+      <c r="EA4" s="3">
+        <f t="shared" ref="EA4" si="45">DZ4+1</f>
+        <v>45505</v>
+      </c>
+      <c r="EB4" s="3">
+        <f t="shared" ref="EB4" si="46">EA4+1</f>
+        <v>45506</v>
+      </c>
+      <c r="EC4" s="3">
+        <f t="shared" ref="EC4" si="47">EB4+1</f>
+        <v>45507</v>
+      </c>
+      <c r="ED4" s="3">
+        <f t="shared" ref="ED4" si="48">EC4+1</f>
+        <v>45508</v>
+      </c>
+      <c r="EE4" s="3">
+        <f t="shared" ref="EE4" si="49">ED4+1</f>
+        <v>45509</v>
+      </c>
+      <c r="EF4" s="3">
+        <f t="shared" ref="EF4" si="50">EE4+1</f>
+        <v>45510</v>
+      </c>
+      <c r="EG4" s="3">
+        <f t="shared" ref="EG4" si="51">EF4+1</f>
+        <v>45511</v>
+      </c>
+      <c r="EH4" s="3">
+        <f t="shared" ref="EH4" si="52">EG4+1</f>
+        <v>45512</v>
+      </c>
+      <c r="EI4" s="3">
+        <f t="shared" ref="EI4" si="53">EH4+1</f>
+        <v>45513</v>
+      </c>
+      <c r="EJ4" s="3">
+        <f t="shared" ref="EJ4" si="54">EI4+1</f>
+        <v>45514</v>
+      </c>
+      <c r="EK4" s="3">
+        <f t="shared" ref="EK4" si="55">EJ4+1</f>
+        <v>45515</v>
+      </c>
+      <c r="EL4" s="3">
+        <f t="shared" ref="EL4" si="56">EK4+1</f>
+        <v>45516</v>
+      </c>
+      <c r="EM4" s="3">
+        <f t="shared" ref="EM4" si="57">EL4+1</f>
+        <v>45517</v>
+      </c>
+      <c r="EN4" s="3">
+        <f t="shared" ref="EN4" si="58">EM4+1</f>
+        <v>45518</v>
+      </c>
+      <c r="EO4" s="3">
+        <f t="shared" ref="EO4" si="59">EN4+1</f>
+        <v>45519</v>
+      </c>
+      <c r="EP4" s="3">
+        <f t="shared" ref="EP4" si="60">EO4+1</f>
+        <v>45520</v>
+      </c>
+      <c r="EQ4" s="3">
+        <f t="shared" ref="EQ4" si="61">EP4+1</f>
+        <v>45521</v>
+      </c>
+      <c r="ER4" s="3">
+        <f t="shared" ref="ER4" si="62">EQ4+1</f>
+        <v>45522</v>
+      </c>
+      <c r="ES4" s="3">
+        <f t="shared" ref="ES4" si="63">ER4+1</f>
+        <v>45523</v>
+      </c>
+      <c r="ET4" s="3">
+        <f t="shared" ref="ET4" si="64">ES4+1</f>
+        <v>45524</v>
+      </c>
+      <c r="EU4" s="3">
+        <f t="shared" ref="EU4" si="65">ET4+1</f>
+        <v>45525</v>
+      </c>
     </row>
-    <row r="5" spans="1:92" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:151" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="15">
         <v>45380</v>
       </c>
-      <c r="D5" s="2">
-        <v>45450</v>
+      <c r="D5" s="15">
+        <v>45525</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" ref="E5:E11" si="1">D5-C5</f>
-        <v>70</v>
+        <f t="shared" ref="E5:E12" si="66">D5-C5</f>
+        <v>145</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -884,28 +1185,87 @@
       <c r="CF5" s="4"/>
       <c r="CG5" s="4"/>
       <c r="CH5" s="4"/>
-      <c r="CI5" s="6"/>
-      <c r="CJ5" s="6"/>
-      <c r="CK5" s="6"/>
-      <c r="CL5" s="6"/>
-      <c r="CM5" s="6"/>
-      <c r="CN5" s="6"/>
+      <c r="CI5" s="4"/>
+      <c r="CJ5" s="4"/>
+      <c r="CK5" s="4"/>
+      <c r="CL5" s="4"/>
+      <c r="CM5" s="4"/>
+      <c r="CN5" s="4"/>
+      <c r="CO5" s="4"/>
+      <c r="CP5" s="4"/>
+      <c r="CQ5" s="4"/>
+      <c r="CR5" s="4"/>
+      <c r="CS5" s="4"/>
+      <c r="CT5" s="4"/>
+      <c r="CU5" s="4"/>
+      <c r="CV5" s="4"/>
+      <c r="CW5" s="4"/>
+      <c r="CX5" s="4"/>
+      <c r="CY5" s="4"/>
+      <c r="CZ5" s="4"/>
+      <c r="DA5" s="4"/>
+      <c r="DB5" s="4"/>
+      <c r="DC5" s="4"/>
+      <c r="DD5" s="4"/>
+      <c r="DE5" s="4"/>
+      <c r="DF5" s="4"/>
+      <c r="DG5" s="4"/>
+      <c r="DH5" s="4"/>
+      <c r="DI5" s="4"/>
+      <c r="DJ5" s="4"/>
+      <c r="DK5" s="4"/>
+      <c r="DL5" s="4"/>
+      <c r="DM5" s="4"/>
+      <c r="DN5" s="4"/>
+      <c r="DO5" s="4"/>
+      <c r="DP5" s="4"/>
+      <c r="DQ5" s="4"/>
+      <c r="DR5" s="4"/>
+      <c r="DS5" s="4"/>
+      <c r="DT5" s="4"/>
+      <c r="DU5" s="4"/>
+      <c r="DV5" s="4"/>
+      <c r="DW5" s="4"/>
+      <c r="DX5" s="4"/>
+      <c r="DY5" s="4"/>
+      <c r="DZ5" s="4"/>
+      <c r="EA5" s="4"/>
+      <c r="EB5" s="4"/>
+      <c r="EC5" s="4"/>
+      <c r="ED5" s="4"/>
+      <c r="EE5" s="4"/>
+      <c r="EF5" s="4"/>
+      <c r="EG5" s="4"/>
+      <c r="EH5" s="4"/>
+      <c r="EI5" s="4"/>
+      <c r="EJ5" s="4"/>
+      <c r="EK5" s="4"/>
+      <c r="EL5" s="4"/>
+      <c r="EM5" s="4"/>
+      <c r="EN5" s="4"/>
+      <c r="EO5" s="4"/>
+      <c r="EP5" s="4"/>
+      <c r="EQ5" s="4"/>
+      <c r="ER5" s="4"/>
+      <c r="ES5" s="4"/>
+      <c r="ET5" s="4"/>
+      <c r="EU5" s="4"/>
     </row>
-    <row r="6" spans="1:92" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:151" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="15">
         <v>45415</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="15">
         <v>45422</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="66"/>
         <v>7</v>
       </c>
       <c r="M6" s="6"/>
@@ -989,21 +1349,21 @@
       <c r="CM6" s="6"/>
       <c r="CN6" s="6"/>
     </row>
-    <row r="7" spans="1:92" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:151" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="15">
         <v>45422</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="15">
         <v>45429</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="66"/>
         <v>7</v>
       </c>
       <c r="F7" s="3"/>
@@ -1022,68 +1382,68 @@
       <c r="BB7" s="8"/>
       <c r="BC7" s="8"/>
     </row>
-    <row r="8" spans="1:92" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:151" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="15">
         <v>45432</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="15">
         <v>45450</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="66"/>
         <v>18</v>
       </c>
-      <c r="BF8" s="9"/>
-      <c r="BG8" s="9"/>
-      <c r="BH8" s="9"/>
-      <c r="BI8" s="9"/>
-      <c r="BJ8" s="9"/>
-      <c r="BK8" s="9"/>
-      <c r="BL8" s="9"/>
-      <c r="BM8" s="9"/>
-      <c r="BN8" s="9"/>
-      <c r="BO8" s="9"/>
-      <c r="BP8" s="9"/>
-      <c r="BQ8" s="9"/>
-      <c r="BR8" s="9"/>
+      <c r="BF8" s="1"/>
+      <c r="BG8" s="1"/>
+      <c r="BH8" s="1"/>
+      <c r="BI8" s="13"/>
+      <c r="BJ8" s="13"/>
+      <c r="BK8" s="13"/>
+      <c r="BL8" s="13"/>
+      <c r="BM8" s="13"/>
+      <c r="BN8" s="13"/>
+      <c r="BO8" s="13"/>
+      <c r="BP8" s="13"/>
+      <c r="BQ8" s="13"/>
+      <c r="BR8" s="13"/>
       <c r="BS8" s="9"/>
       <c r="BT8" s="9"/>
       <c r="BU8" s="9"/>
       <c r="BV8" s="9"/>
       <c r="BW8" s="9"/>
       <c r="BX8" s="9"/>
-      <c r="BY8" s="9"/>
-      <c r="BZ8" s="9"/>
-      <c r="CA8" s="9"/>
-      <c r="CB8" s="9"/>
-      <c r="CC8" s="9"/>
-      <c r="CD8" s="9"/>
-      <c r="CE8" s="9"/>
-      <c r="CF8" s="9"/>
-      <c r="CG8" s="9"/>
-      <c r="CH8" s="9"/>
+      <c r="BY8" s="13"/>
+      <c r="BZ8" s="13"/>
+      <c r="CA8" s="13"/>
+      <c r="CB8" s="13"/>
+      <c r="CC8" s="13"/>
+      <c r="CD8" s="13"/>
+      <c r="CE8" s="13"/>
+      <c r="CF8" s="13"/>
+      <c r="CG8" s="13"/>
+      <c r="CH8" s="13"/>
     </row>
-    <row r="9" spans="1:92" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:151" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="15">
         <v>45387</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="15">
         <v>45401</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="66"/>
         <v>14</v>
       </c>
       <c r="M9" s="10"/>
@@ -1101,27 +1461,27 @@
       <c r="Y9" s="10"/>
       <c r="Z9" s="10"/>
       <c r="AA9" s="10"/>
+      <c r="AB9" s="10"/>
+      <c r="AC9" s="10"/>
+      <c r="AD9" s="10"/>
     </row>
-    <row r="10" spans="1:92" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:151" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="15">
         <v>45402</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="15">
         <v>45416</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="66"/>
         <v>14</v>
       </c>
-      <c r="AB10" s="11"/>
-      <c r="AC10" s="11"/>
-      <c r="AD10" s="11"/>
       <c r="AE10" s="11"/>
       <c r="AF10" s="11"/>
       <c r="AG10" s="11"/>
@@ -1134,39 +1494,189 @@
       <c r="AN10" s="11"/>
       <c r="AO10" s="11"/>
       <c r="AP10" s="11"/>
+      <c r="AQ10" s="11"/>
+      <c r="AR10" s="11"/>
+      <c r="AS10" s="11"/>
     </row>
-    <row r="11" spans="1:92" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:151" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="15">
         <v>45417</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="15">
         <v>45431</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="66"/>
         <v>14</v>
       </c>
-      <c r="AQ11" s="12"/>
-      <c r="AR11" s="12"/>
-      <c r="AS11" s="12"/>
-      <c r="AT11" s="12"/>
-      <c r="AU11" s="12"/>
-      <c r="AV11" s="12"/>
-      <c r="AW11" s="12"/>
-      <c r="AX11" s="12"/>
-      <c r="AY11" s="12"/>
-      <c r="AZ11" s="12"/>
-      <c r="BA11" s="12"/>
-      <c r="BB11" s="12"/>
-      <c r="BC11" s="12"/>
-      <c r="BD11" s="12"/>
-      <c r="BE11" s="12"/>
+      <c r="BS11" s="12"/>
+      <c r="BT11" s="12"/>
+      <c r="BU11" s="12"/>
+      <c r="BV11" s="12"/>
+      <c r="BW11" s="12"/>
+      <c r="BX11" s="12"/>
+      <c r="BY11" s="13"/>
+      <c r="BZ11" s="13"/>
+      <c r="CA11" s="13"/>
+      <c r="CB11" s="13"/>
+      <c r="CC11" s="13"/>
+      <c r="CD11" s="13"/>
+      <c r="CE11" s="13"/>
+      <c r="CF11" s="13"/>
+      <c r="CG11" s="13"/>
+    </row>
+    <row r="12" spans="1:151" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="15">
+        <v>45451</v>
+      </c>
+      <c r="D12" s="15">
+        <v>45465</v>
+      </c>
+      <c r="E12" s="1">
+        <f>D12-C12</f>
+        <v>14</v>
+      </c>
+      <c r="BY12" s="14"/>
+      <c r="BZ12" s="14"/>
+      <c r="CA12" s="14"/>
+      <c r="CB12" s="14"/>
+      <c r="CC12" s="14"/>
+      <c r="CD12" s="14"/>
+      <c r="CE12" s="14"/>
+      <c r="CF12" s="14"/>
+      <c r="CG12" s="14"/>
+      <c r="CH12" s="14"/>
+      <c r="CI12" s="14"/>
+      <c r="CJ12" s="14"/>
+      <c r="CK12" s="14"/>
+      <c r="CL12" s="14"/>
+      <c r="CM12" s="14"/>
+    </row>
+    <row r="13" spans="1:151" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="15">
+        <v>45466</v>
+      </c>
+      <c r="D13" s="15">
+        <v>45480</v>
+      </c>
+      <c r="E13" s="1">
+        <f>D13-C13</f>
+        <v>14</v>
+      </c>
+      <c r="CN13" s="16"/>
+      <c r="CO13" s="16"/>
+      <c r="CP13" s="16"/>
+      <c r="CQ13" s="16"/>
+      <c r="CR13" s="16"/>
+      <c r="CS13" s="16"/>
+      <c r="CT13" s="16"/>
+      <c r="CU13" s="16"/>
+      <c r="CV13" s="16"/>
+      <c r="CW13" s="16"/>
+      <c r="CX13" s="16"/>
+      <c r="CY13" s="16"/>
+      <c r="CZ13" s="16"/>
+      <c r="DA13" s="16"/>
+      <c r="DB13" s="16"/>
+    </row>
+    <row r="14" spans="1:151" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="15">
+        <v>45481</v>
+      </c>
+      <c r="D14" s="15">
+        <v>45495</v>
+      </c>
+      <c r="E14" s="1">
+        <f>D14-C14</f>
+        <v>14</v>
+      </c>
+      <c r="DC14" s="17"/>
+      <c r="DD14" s="17"/>
+      <c r="DE14" s="17"/>
+      <c r="DF14" s="17"/>
+      <c r="DG14" s="17"/>
+      <c r="DH14" s="17"/>
+      <c r="DI14" s="17"/>
+      <c r="DJ14" s="17"/>
+      <c r="DK14" s="17"/>
+      <c r="DL14" s="17"/>
+      <c r="DM14" s="17"/>
+      <c r="DN14" s="17"/>
+      <c r="DO14" s="17"/>
+      <c r="DP14" s="17"/>
+      <c r="DQ14" s="17"/>
+    </row>
+    <row r="15" spans="1:151" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="15">
+        <v>45496</v>
+      </c>
+      <c r="D15" s="15">
+        <v>45525</v>
+      </c>
+      <c r="E15" s="1">
+        <f>D15-C15</f>
+        <v>29</v>
+      </c>
+      <c r="DR15" s="18"/>
+      <c r="DS15" s="18"/>
+      <c r="DT15" s="18"/>
+      <c r="DU15" s="18"/>
+      <c r="DV15" s="18"/>
+      <c r="DW15" s="18"/>
+      <c r="DX15" s="18"/>
+      <c r="DY15" s="18"/>
+      <c r="DZ15" s="18"/>
+      <c r="EA15" s="18"/>
+      <c r="EB15" s="18"/>
+      <c r="EC15" s="18"/>
+      <c r="ED15" s="18"/>
+      <c r="EE15" s="18"/>
+      <c r="EF15" s="18"/>
+      <c r="EG15" s="18"/>
+      <c r="EH15" s="18"/>
+      <c r="EI15" s="18"/>
+      <c r="EJ15" s="18"/>
+      <c r="EK15" s="18"/>
+      <c r="EL15" s="18"/>
+      <c r="EM15" s="18"/>
+      <c r="EN15" s="18"/>
+      <c r="EO15" s="18"/>
+      <c r="EP15" s="18"/>
+      <c r="EQ15" s="18"/>
+      <c r="ER15" s="18"/>
+      <c r="ES15" s="18"/>
+      <c r="ET15" s="18"/>
+      <c r="EU15" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Eric for class (#41)
* auto pipeline up to interact(), need some more simplification for later edits

* updated doc for class submission

* new adjusted Gannt chart

* Add files via upload
</commit_message>
<xml_diff>
--- a/doc/project Gannt Chart.xlsx
+++ b/doc/project Gannt Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric Xue\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric Xue\Desktop\UW Seattle\March quater\data sci cap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2C110B-7A21-4B21-A7F2-55797E74ECDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CE45B4-4699-40C7-829A-9CCF2F454EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="585" windowWidth="18000" windowHeight="9165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Project name</t>
   </si>
@@ -90,6 +90,18 @@
   </si>
   <si>
     <t>debugg before final submission</t>
+  </si>
+  <si>
+    <t>unit tests</t>
+  </si>
+  <si>
+    <t>package the project</t>
+  </si>
+  <si>
+    <t>feature: file selection interface</t>
+  </si>
+  <si>
+    <t>tutorial notebook</t>
   </si>
 </sst>
 </file>
@@ -114,7 +126,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,6 +169,30 @@
         <bgColor rgb="FFF6B26B"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -170,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -186,12 +222,24 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF9966FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -404,23 +452,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:CN11"/>
+  <dimension ref="A1:EU15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="CV5" sqref="CV5:EU5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
     <col min="3" max="3" width="8.140625" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" customWidth="1"/>
     <col min="5" max="5" width="5.5703125" customWidth="1"/>
-    <col min="6" max="92" width="2.5703125" customWidth="1"/>
+    <col min="6" max="151" width="2.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:92" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:151" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -434,7 +482,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:92" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:151" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C2" s="2">
         <v>45380</v>
       </c>
@@ -442,7 +490,7 @@
         <v>45450</v>
       </c>
     </row>
-    <row r="4" spans="1:92" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:151" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -782,26 +830,124 @@
         <f t="shared" si="0"/>
         <v>45460</v>
       </c>
-      <c r="CI4" s="3"/>
-      <c r="CJ4" s="3"/>
-      <c r="CK4" s="3"/>
-      <c r="CL4" s="3"/>
-      <c r="CM4" s="3"/>
-      <c r="CN4" s="3"/>
+      <c r="CI4" s="3">
+        <f t="shared" ref="CI4" si="1">CH4+1</f>
+        <v>45461</v>
+      </c>
+      <c r="CJ4" s="3">
+        <f t="shared" ref="CJ4" si="2">CI4+1</f>
+        <v>45462</v>
+      </c>
+      <c r="CK4" s="3">
+        <f t="shared" ref="CK4" si="3">CJ4+1</f>
+        <v>45463</v>
+      </c>
+      <c r="CL4" s="3">
+        <f t="shared" ref="CL4" si="4">CK4+1</f>
+        <v>45464</v>
+      </c>
+      <c r="CM4" s="3">
+        <f t="shared" ref="CM4" si="5">CL4+1</f>
+        <v>45465</v>
+      </c>
+      <c r="CN4" s="3">
+        <f t="shared" ref="CN4" si="6">CM4+1</f>
+        <v>45466</v>
+      </c>
+      <c r="CO4" s="3">
+        <f t="shared" ref="CO4" si="7">CN4+1</f>
+        <v>45467</v>
+      </c>
+      <c r="CP4" s="3">
+        <f t="shared" ref="CP4" si="8">CO4+1</f>
+        <v>45468</v>
+      </c>
+      <c r="CQ4" s="3">
+        <f t="shared" ref="CQ4" si="9">CP4+1</f>
+        <v>45469</v>
+      </c>
+      <c r="CR4" s="3">
+        <f t="shared" ref="CR4" si="10">CQ4+1</f>
+        <v>45470</v>
+      </c>
+      <c r="CS4" s="3">
+        <f t="shared" ref="CS4" si="11">CR4+1</f>
+        <v>45471</v>
+      </c>
+      <c r="CT4" s="3">
+        <f t="shared" ref="CT4" si="12">CS4+1</f>
+        <v>45472</v>
+      </c>
+      <c r="CU4" s="3">
+        <f t="shared" ref="CU4" si="13">CT4+1</f>
+        <v>45473</v>
+      </c>
+      <c r="CV4" s="3"/>
+      <c r="CW4" s="3"/>
+      <c r="CX4" s="3"/>
+      <c r="CY4" s="3"/>
+      <c r="CZ4" s="3"/>
+      <c r="DA4" s="3"/>
+      <c r="DB4" s="3"/>
+      <c r="DC4" s="3"/>
+      <c r="DD4" s="3"/>
+      <c r="DE4" s="3"/>
+      <c r="DF4" s="3"/>
+      <c r="DG4" s="3"/>
+      <c r="DH4" s="3"/>
+      <c r="DI4" s="3"/>
+      <c r="DJ4" s="3"/>
+      <c r="DK4" s="3"/>
+      <c r="DL4" s="3"/>
+      <c r="DM4" s="3"/>
+      <c r="DN4" s="3"/>
+      <c r="DO4" s="3"/>
+      <c r="DP4" s="3"/>
+      <c r="DQ4" s="3"/>
+      <c r="DR4" s="3"/>
+      <c r="DS4" s="3"/>
+      <c r="DT4" s="3"/>
+      <c r="DU4" s="3"/>
+      <c r="DV4" s="3"/>
+      <c r="DW4" s="3"/>
+      <c r="DX4" s="3"/>
+      <c r="DY4" s="3"/>
+      <c r="DZ4" s="3"/>
+      <c r="EA4" s="3"/>
+      <c r="EB4" s="3"/>
+      <c r="EC4" s="3"/>
+      <c r="ED4" s="3"/>
+      <c r="EE4" s="3"/>
+      <c r="EF4" s="3"/>
+      <c r="EG4" s="3"/>
+      <c r="EH4" s="3"/>
+      <c r="EI4" s="3"/>
+      <c r="EJ4" s="3"/>
+      <c r="EK4" s="3"/>
+      <c r="EL4" s="3"/>
+      <c r="EM4" s="3"/>
+      <c r="EN4" s="3"/>
+      <c r="EO4" s="3"/>
+      <c r="EP4" s="3"/>
+      <c r="EQ4" s="3"/>
+      <c r="ER4" s="3"/>
+      <c r="ES4" s="3"/>
+      <c r="ET4" s="3"/>
+      <c r="EU4" s="3"/>
     </row>
-    <row r="5" spans="1:92" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:151" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="14">
         <v>45380</v>
       </c>
-      <c r="D5" s="2">
-        <v>45450</v>
+      <c r="D5" s="14">
+        <v>45525</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" ref="E5:E11" si="1">D5-C5</f>
-        <v>70</v>
+        <f t="shared" ref="E5:E11" si="14">D5-C5</f>
+        <v>145</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -884,28 +1030,87 @@
       <c r="CF5" s="4"/>
       <c r="CG5" s="4"/>
       <c r="CH5" s="4"/>
-      <c r="CI5" s="6"/>
-      <c r="CJ5" s="6"/>
-      <c r="CK5" s="6"/>
-      <c r="CL5" s="6"/>
-      <c r="CM5" s="6"/>
-      <c r="CN5" s="6"/>
+      <c r="CI5" s="4"/>
+      <c r="CJ5" s="4"/>
+      <c r="CK5" s="4"/>
+      <c r="CL5" s="4"/>
+      <c r="CM5" s="4"/>
+      <c r="CN5" s="4"/>
+      <c r="CO5" s="4"/>
+      <c r="CP5" s="4"/>
+      <c r="CQ5" s="4"/>
+      <c r="CR5" s="4"/>
+      <c r="CS5" s="4"/>
+      <c r="CT5" s="4"/>
+      <c r="CU5" s="4"/>
+      <c r="CV5" s="19"/>
+      <c r="CW5" s="19"/>
+      <c r="CX5" s="19"/>
+      <c r="CY5" s="19"/>
+      <c r="CZ5" s="19"/>
+      <c r="DA5" s="19"/>
+      <c r="DB5" s="19"/>
+      <c r="DC5" s="19"/>
+      <c r="DD5" s="19"/>
+      <c r="DE5" s="19"/>
+      <c r="DF5" s="19"/>
+      <c r="DG5" s="19"/>
+      <c r="DH5" s="19"/>
+      <c r="DI5" s="19"/>
+      <c r="DJ5" s="19"/>
+      <c r="DK5" s="19"/>
+      <c r="DL5" s="19"/>
+      <c r="DM5" s="19"/>
+      <c r="DN5" s="19"/>
+      <c r="DO5" s="19"/>
+      <c r="DP5" s="19"/>
+      <c r="DQ5" s="19"/>
+      <c r="DR5" s="19"/>
+      <c r="DS5" s="19"/>
+      <c r="DT5" s="19"/>
+      <c r="DU5" s="19"/>
+      <c r="DV5" s="19"/>
+      <c r="DW5" s="19"/>
+      <c r="DX5" s="19"/>
+      <c r="DY5" s="19"/>
+      <c r="DZ5" s="19"/>
+      <c r="EA5" s="19"/>
+      <c r="EB5" s="19"/>
+      <c r="EC5" s="19"/>
+      <c r="ED5" s="19"/>
+      <c r="EE5" s="19"/>
+      <c r="EF5" s="19"/>
+      <c r="EG5" s="19"/>
+      <c r="EH5" s="19"/>
+      <c r="EI5" s="19"/>
+      <c r="EJ5" s="19"/>
+      <c r="EK5" s="19"/>
+      <c r="EL5" s="19"/>
+      <c r="EM5" s="19"/>
+      <c r="EN5" s="19"/>
+      <c r="EO5" s="19"/>
+      <c r="EP5" s="19"/>
+      <c r="EQ5" s="19"/>
+      <c r="ER5" s="19"/>
+      <c r="ES5" s="19"/>
+      <c r="ET5" s="19"/>
+      <c r="EU5" s="19"/>
     </row>
-    <row r="6" spans="1:92" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:151" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="14">
         <v>45415</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="14">
         <v>45422</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="M6" s="6"/>
@@ -989,21 +1194,21 @@
       <c r="CM6" s="6"/>
       <c r="CN6" s="6"/>
     </row>
-    <row r="7" spans="1:92" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:151" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="14">
         <v>45422</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="14">
         <v>45429</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="F7" s="3"/>
@@ -1022,68 +1227,68 @@
       <c r="BB7" s="8"/>
       <c r="BC7" s="8"/>
     </row>
-    <row r="8" spans="1:92" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:151" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="14">
         <v>45432</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="14">
         <v>45450</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>18</v>
       </c>
-      <c r="BF8" s="9"/>
-      <c r="BG8" s="9"/>
-      <c r="BH8" s="9"/>
-      <c r="BI8" s="9"/>
-      <c r="BJ8" s="9"/>
-      <c r="BK8" s="9"/>
-      <c r="BL8" s="9"/>
-      <c r="BM8" s="9"/>
-      <c r="BN8" s="9"/>
-      <c r="BO8" s="9"/>
-      <c r="BP8" s="9"/>
-      <c r="BQ8" s="9"/>
-      <c r="BR8" s="9"/>
+      <c r="BF8" s="1"/>
+      <c r="BG8" s="1"/>
+      <c r="BH8" s="1"/>
+      <c r="BI8" s="1"/>
+      <c r="BJ8" s="1"/>
+      <c r="BK8" s="1"/>
+      <c r="BL8" s="1"/>
+      <c r="BM8" s="1"/>
+      <c r="BN8" s="1"/>
+      <c r="BO8" s="1"/>
+      <c r="BP8" s="1"/>
+      <c r="BQ8" s="1"/>
+      <c r="BR8" s="1"/>
       <c r="BS8" s="9"/>
       <c r="BT8" s="9"/>
       <c r="BU8" s="9"/>
       <c r="BV8" s="9"/>
       <c r="BW8" s="9"/>
       <c r="BX8" s="9"/>
-      <c r="BY8" s="9"/>
-      <c r="BZ8" s="9"/>
-      <c r="CA8" s="9"/>
-      <c r="CB8" s="9"/>
-      <c r="CC8" s="9"/>
-      <c r="CD8" s="9"/>
-      <c r="CE8" s="9"/>
-      <c r="CF8" s="9"/>
-      <c r="CG8" s="9"/>
-      <c r="CH8" s="9"/>
+      <c r="BY8" s="1"/>
+      <c r="BZ8" s="1"/>
+      <c r="CA8" s="1"/>
+      <c r="CB8" s="1"/>
+      <c r="CC8" s="1"/>
+      <c r="CD8" s="1"/>
+      <c r="CE8" s="1"/>
+      <c r="CF8" s="1"/>
+      <c r="CG8" s="1"/>
+      <c r="CH8" s="1"/>
     </row>
-    <row r="9" spans="1:92" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:151" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="14">
         <v>45387</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="14">
         <v>45401</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>14</v>
       </c>
       <c r="M9" s="10"/>
@@ -1101,27 +1306,27 @@
       <c r="Y9" s="10"/>
       <c r="Z9" s="10"/>
       <c r="AA9" s="10"/>
+      <c r="AB9" s="10"/>
+      <c r="AC9" s="10"/>
+      <c r="AD9" s="10"/>
     </row>
-    <row r="10" spans="1:92" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:151" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="14">
         <v>45402</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="14">
         <v>45416</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>14</v>
       </c>
-      <c r="AB10" s="11"/>
-      <c r="AC10" s="11"/>
-      <c r="AD10" s="11"/>
       <c r="AE10" s="11"/>
       <c r="AF10" s="11"/>
       <c r="AG10" s="11"/>
@@ -1134,39 +1339,198 @@
       <c r="AN10" s="11"/>
       <c r="AO10" s="11"/>
       <c r="AP10" s="11"/>
+      <c r="AQ10" s="11"/>
+      <c r="AR10" s="11"/>
+      <c r="AS10" s="11"/>
     </row>
-    <row r="11" spans="1:92" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:151" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="14">
         <v>45417</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="14">
         <v>45431</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="14"/>
         <v>14</v>
       </c>
-      <c r="AQ11" s="12"/>
-      <c r="AR11" s="12"/>
-      <c r="AS11" s="12"/>
-      <c r="AT11" s="12"/>
-      <c r="AU11" s="12"/>
-      <c r="AV11" s="12"/>
-      <c r="AW11" s="12"/>
-      <c r="AX11" s="12"/>
-      <c r="AY11" s="12"/>
-      <c r="AZ11" s="12"/>
-      <c r="BA11" s="12"/>
-      <c r="BB11" s="12"/>
-      <c r="BC11" s="12"/>
-      <c r="BD11" s="12"/>
-      <c r="BE11" s="12"/>
+      <c r="BS11" s="12"/>
+      <c r="BT11" s="12"/>
+      <c r="BU11" s="12"/>
+      <c r="BV11" s="12"/>
+      <c r="BW11" s="12"/>
+      <c r="BX11" s="12"/>
+      <c r="BY11" s="1"/>
+      <c r="BZ11" s="1"/>
+      <c r="CA11" s="1"/>
+      <c r="CB11" s="1"/>
+      <c r="CC11" s="1"/>
+      <c r="CD11" s="1"/>
+      <c r="CE11" s="1"/>
+      <c r="CF11" s="1"/>
+      <c r="CG11" s="1"/>
+    </row>
+    <row r="12" spans="1:151" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="14">
+        <v>45451</v>
+      </c>
+      <c r="D12" s="14">
+        <v>45458</v>
+      </c>
+      <c r="E12" s="1">
+        <f>D12-C12</f>
+        <v>7</v>
+      </c>
+      <c r="BY12" s="13"/>
+      <c r="BZ12" s="13"/>
+      <c r="CA12" s="13"/>
+      <c r="CB12" s="13"/>
+      <c r="CC12" s="13"/>
+      <c r="CD12" s="13"/>
+      <c r="CE12" s="13"/>
+      <c r="CF12" s="13"/>
+      <c r="CG12" s="18"/>
+      <c r="CH12" s="18"/>
+      <c r="CI12" s="18"/>
+      <c r="CJ12" s="18"/>
+      <c r="CK12" s="18"/>
+      <c r="CL12" s="18"/>
+      <c r="CM12" s="18"/>
+    </row>
+    <row r="13" spans="1:151" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="14">
+        <v>45459</v>
+      </c>
+      <c r="D13" s="14">
+        <v>45473</v>
+      </c>
+      <c r="E13" s="1">
+        <f>D13-C13</f>
+        <v>14</v>
+      </c>
+      <c r="CG13" s="15"/>
+      <c r="CH13" s="15"/>
+      <c r="CI13" s="15"/>
+      <c r="CJ13" s="15"/>
+      <c r="CK13" s="15"/>
+      <c r="CL13" s="15"/>
+      <c r="CM13" s="15"/>
+      <c r="CN13" s="15"/>
+      <c r="CO13" s="15"/>
+      <c r="CP13" s="15"/>
+      <c r="CQ13" s="15"/>
+      <c r="CR13" s="15"/>
+      <c r="CS13" s="15"/>
+      <c r="CT13" s="15"/>
+      <c r="CU13" s="15"/>
+    </row>
+    <row r="14" spans="1:151" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="14">
+        <v>45459</v>
+      </c>
+      <c r="D14" s="14">
+        <v>45473</v>
+      </c>
+      <c r="E14" s="1">
+        <f>D14-C14</f>
+        <v>14</v>
+      </c>
+      <c r="CG14" s="16"/>
+      <c r="CH14" s="16"/>
+      <c r="CI14" s="16"/>
+      <c r="CJ14" s="16"/>
+      <c r="CK14" s="16"/>
+      <c r="CL14" s="16"/>
+      <c r="CM14" s="16"/>
+      <c r="CN14" s="16"/>
+      <c r="CO14" s="16"/>
+      <c r="CP14" s="16"/>
+      <c r="CQ14" s="16"/>
+      <c r="CR14" s="16"/>
+      <c r="CS14" s="16"/>
+      <c r="CT14" s="16"/>
+      <c r="CU14" s="16"/>
+    </row>
+    <row r="15" spans="1:151" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="14">
+        <v>45459</v>
+      </c>
+      <c r="D15" s="14">
+        <v>45473</v>
+      </c>
+      <c r="E15" s="1">
+        <f>D15-C15</f>
+        <v>14</v>
+      </c>
+      <c r="CG15" s="17"/>
+      <c r="CH15" s="17"/>
+      <c r="CI15" s="17"/>
+      <c r="CJ15" s="17"/>
+      <c r="CK15" s="17"/>
+      <c r="CL15" s="17"/>
+      <c r="CM15" s="17"/>
+      <c r="CN15" s="17"/>
+      <c r="CO15" s="17"/>
+      <c r="CP15" s="17"/>
+      <c r="CQ15" s="17"/>
+      <c r="CR15" s="17"/>
+      <c r="CS15" s="17"/>
+      <c r="CT15" s="17"/>
+      <c r="CU15" s="17"/>
+      <c r="DX15" s="18"/>
+      <c r="DY15" s="18"/>
+      <c r="DZ15" s="18"/>
+      <c r="EA15" s="18"/>
+      <c r="EB15" s="18"/>
+      <c r="EC15" s="18"/>
+      <c r="ED15" s="18"/>
+      <c r="EE15" s="18"/>
+      <c r="EF15" s="18"/>
+      <c r="EG15" s="18"/>
+      <c r="EH15" s="18"/>
+      <c r="EI15" s="18"/>
+      <c r="EJ15" s="18"/>
+      <c r="EK15" s="18"/>
+      <c r="EL15" s="18"/>
+      <c r="EM15" s="18"/>
+      <c r="EN15" s="18"/>
+      <c r="EO15" s="18"/>
+      <c r="EP15" s="18"/>
+      <c r="EQ15" s="18"/>
+      <c r="ER15" s="18"/>
+      <c r="ES15" s="18"/>
+      <c r="ET15" s="18"/>
+      <c r="EU15" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>